<commit_message>
hw 6 prelim finish
</commit_message>
<xml_diff>
--- a/hws/hw06/q1-output.xlsx
+++ b/hws/hw06/q1-output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aelhabr\Documents\projects\isye-6420\hws\hw06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA6BD1A-86BB-4B3B-B777-FB3E5474B31F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE551A6E-184D-4259-9496-7A6B12189618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9990" yWindow="1650" windowWidth="16305" windowHeight="11505" xr2:uid="{CCB633D7-E740-4986-8EC1-2E25EE92EC97}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CCB633D7-E740-4986-8EC1-2E25EE92EC97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1150,7 +1150,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51DD2A8-3CDF-423D-BA7F-5B97F7D94599}">
   <dimension ref="A1:I247"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:S1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>